<commit_message>
add opportunity to choose time space in report;
</commit_message>
<xml_diff>
--- a/excele_reporter/Срез 30 мин E+.xlsx
+++ b/excele_reporter/Срез 30 мин E+.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Office CE301..Office CE301" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="ООО &quot;Сервовит&quot;..ООО &quot;Сервовит&quot;" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="КаргоПромСтрой..КаргоПромСтрой" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Office SS301..Office SS301" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -50328,4 +50329,2084 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C145"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Датчик Office SS301</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>05:30-06:00</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>06:00-06:30</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>06:30-07:00</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>07:00-07:30</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>07:30-08:00</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:00-08:30</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>08:30-09:00</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:00-09:30</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>09:30-10:00</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>10:00-10:30</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>10:30-11:00</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11:00-11:30</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:30-12:00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>12:00-12:30</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>12:30-13:00</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:00-13:30</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13:30-14:00</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>14:00-14:30</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:30-15:00</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>15:00-15:30</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>15:30-16:00</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>16:00-16:30</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>16:30-17:00</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>17:00-17:30</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>17:30-18:00</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>18:00-18:30</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>18:30-19:00</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>19:00-19:30</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>19:30-20:00</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>20:00-20:30</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>20:30-21:00</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>21:00-21:30</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>21:30-22:00</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>22:00-22:30</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>22:30-23:00</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>23:00-23:30</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2023-02-26</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>23:30-24:00</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>00:00-00:30</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>00:30-01:00</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>01:00-01:30</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>01:30-02:00</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>02:00-02:30</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>02:30-03:00</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>03:00-03:30</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>03:30-04:00</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>04:00-04:30</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>04:30-05:00</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>05:00-05:30</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>05:30-06:00</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>06:00-06:30</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>06:30-07:00</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>07:00-07:30</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>07:30-08:00</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>08:00-08:30</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>08:30-09:00</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>09:00-09:30</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>09:30-10:00</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>10:00-10:30</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>10:30-11:00</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>11:00-11:30</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>11:30-12:00</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>12:00-12:30</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>12:30-13:00</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>13:00-13:30</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>13:30-14:00</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>14:00-14:30</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>14:30-15:00</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>15:00-15:30</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>15:30-16:00</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>16:00-16:30</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>16:30-17:00</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>17:00-17:30</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>17:30-18:00</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>18:00-18:30</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>18:30-19:00</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>19:00-19:30</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>19:30-20:00</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>20:00-20:30</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>20:30-21:00</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>21:00-21:30</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>21:30-22:00</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>22:00-22:30</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>22:30-23:00</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>23:00-23:30</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>23:30-24:00</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>00:00-00:30</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>00:30-01:00</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>01:00-01:30</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>01:30-02:00</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>02:00-02:30</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>02:30-03:00</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>03:00-03:30</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>03:30-04:00</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>04:00-04:30</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>04:30-05:00</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>05:00-05:30</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>05:30-06:00</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>06:00-06:30</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>06:30-07:00</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>07:00-07:30</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>07:30-08:00</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>08:00-08:30</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>08:30-09:00</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>09:00-09:30</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>09:30-10:00</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>10:00-10:30</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>10:30-11:00</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>11:00-11:30</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>11:30-12:00</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>12:00-12:30</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>12:30-13:00</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>13:00-13:30</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>13:30-14:00</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>14:00-14:30</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>14:30-15:00</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>15:00-15:30</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>15:30-16:00</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>16:00-16:30</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>16:30-17:00</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>17:00-17:30</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr"/>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>17:30-18:00</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr"/>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>18:00-18:30</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr"/>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>18:30-19:00</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr"/>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>19:00-19:30</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr"/>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>19:30-20:00</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr"/>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>20:00-20:30</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr"/>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>20:30-21:00</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr"/>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>21:00-21:30</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr"/>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr"/>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr"/>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add the multiple choice for metters in reporter;
</commit_message>
<xml_diff>
--- a/excele_reporter/Срез 30 мин E+.xlsx
+++ b/excele_reporter/Срез 30 мин E+.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Office CE301..Office CE301" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Office CE301..Office SS301" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C145"/>
+  <dimension ref="A1:D145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>Датчик Office CE301</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Датчик Office SS301</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -458,13 +463,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>00:00-00:30</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.005</v>
       </c>
     </row>
     <row r="3">
@@ -475,13 +483,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>00:30-01:00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>-</t>
         </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.005</v>
       </c>
     </row>
     <row r="4">
@@ -500,6 +511,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D4" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -517,6 +531,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D5" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -534,6 +551,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -551,6 +569,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -568,6 +587,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -585,6 +605,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -602,6 +623,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -619,6 +641,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -636,6 +659,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -653,6 +677,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -670,6 +695,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -687,6 +713,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -704,6 +731,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -721,6 +749,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -738,6 +767,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -755,6 +785,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -772,6 +803,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -789,6 +821,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -806,6 +839,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -823,6 +857,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -840,6 +875,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -857,6 +893,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -874,6 +911,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -891,6 +929,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -908,6 +947,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -925,6 +965,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -942,6 +983,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -959,6 +1001,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -976,6 +1019,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -993,6 +1037,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1010,6 +1055,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1027,6 +1073,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1044,6 +1091,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1061,6 +1109,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1078,6 +1127,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1095,6 +1145,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1112,6 +1163,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1129,6 +1181,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1146,6 +1199,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1163,6 +1217,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1180,6 +1235,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1197,6 +1253,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1214,6 +1271,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D46" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1231,6 +1291,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D47" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1248,6 +1311,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D48" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1265,6 +1331,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D49" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1282,6 +1351,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D50" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1299,6 +1371,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D51" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1316,6 +1391,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D52" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1333,6 +1411,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D53" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1350,6 +1431,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D54" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1367,6 +1451,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D55" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1384,6 +1471,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D56" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1401,6 +1491,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D57" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1418,6 +1511,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D58" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1435,6 +1531,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D59" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1452,6 +1551,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D60" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1469,6 +1571,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D61" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1486,6 +1591,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D62" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1503,6 +1611,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D63" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1520,6 +1631,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D64" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1537,6 +1651,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D65" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1554,6 +1671,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D66" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1571,6 +1691,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D67" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1588,6 +1711,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D68" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1605,6 +1731,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D69" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1622,6 +1751,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D70" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1639,6 +1771,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D71" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1656,6 +1791,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D72" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1673,6 +1811,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D73" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1690,6 +1831,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D74" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1707,6 +1851,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D75" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1724,6 +1871,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D76" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1741,6 +1891,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D77" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1758,6 +1911,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D78" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1775,6 +1931,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D79" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1792,6 +1951,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D80" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1809,6 +1971,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D81" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1826,6 +1991,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D82" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1843,6 +2011,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D83" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1860,6 +2031,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D84" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1877,6 +2051,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D85" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1894,6 +2071,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D86" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1911,6 +2091,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D87" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1928,6 +2111,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D88" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1945,6 +2131,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D89" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1962,6 +2151,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D90" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1979,6 +2171,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D91" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1996,6 +2191,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D92" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2013,6 +2211,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D93" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2030,6 +2231,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D94" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2047,6 +2251,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D95" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2064,6 +2271,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D96" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2081,6 +2291,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D97" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -2098,6 +2311,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D98" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -2115,6 +2331,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D99" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2132,6 +2351,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D100" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -2149,6 +2371,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D101" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -2166,6 +2391,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D102" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -2175,13 +2403,16 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>02:30-03:00</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
           <t>-</t>
         </is>
+      </c>
+      <c r="D103" t="n">
+        <v>0.0075</v>
       </c>
     </row>
     <row r="104">
@@ -2192,13 +2423,16 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>03:00-03:30</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
           <t>-</t>
         </is>
+      </c>
+      <c r="D104" t="n">
+        <v>0.005</v>
       </c>
     </row>
     <row r="105">
@@ -2209,13 +2443,16 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>03:30-04:00</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
           <t>-</t>
         </is>
+      </c>
+      <c r="D105" t="n">
+        <v>0.005</v>
       </c>
     </row>
     <row r="106">
@@ -2226,13 +2463,16 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>04:00-04:30</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
           <t>-</t>
         </is>
+      </c>
+      <c r="D106" t="n">
+        <v>0.005</v>
       </c>
     </row>
     <row r="107">
@@ -2251,6 +2491,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D107" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -2268,6 +2511,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D108" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -2285,6 +2531,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D109" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -2302,6 +2551,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D110" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -2319,6 +2571,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D111" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -2336,6 +2591,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D112" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -2353,6 +2611,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D113" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -2370,6 +2631,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D114" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -2387,6 +2651,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D115" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -2404,6 +2671,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D116" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -2421,6 +2691,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D117" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -2438,6 +2711,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D118" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -2455,6 +2731,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D119" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -2472,6 +2751,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D120" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -2489,6 +2771,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D121" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -2506,6 +2791,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D122" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -2523,6 +2811,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D123" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -2540,6 +2831,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D124" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -2557,6 +2851,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D125" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -2574,6 +2871,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D126" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -2591,6 +2891,9 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D127" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -2608,6 +2911,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -2625,6 +2929,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -2642,6 +2947,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -2659,6 +2965,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -2676,6 +2983,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -2693,6 +3001,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -2710,6 +3019,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -2727,6 +3037,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -2744,6 +3055,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -2761,6 +3073,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -2778,6 +3091,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -2795,6 +3109,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -2812,6 +3127,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -2829,6 +3145,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -2846,6 +3163,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -2863,6 +3181,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -2880,6 +3199,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -2897,6 +3217,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="D145" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add opportunity to rewrite sheet in report if it exists;
</commit_message>
<xml_diff>
--- a/excele_reporter/Срез 30 мин E+.xlsx
+++ b/excele_reporter/Срез 30 мин E+.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Office CE301..Office SS301" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name=" ОАО &quot;ММЗ&quot; №1..1T1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2403,7 +2404,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>02:30-03:00</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2423,7 +2424,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>03:00-03:30</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2443,7 +2444,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>03:30-04:00</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3218,6 +3219,2644 @@
         </is>
       </c>
       <c r="D145" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E97"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Датчик  ОАО "ММЗ" №1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Датчик  ОАО "ММЗ" №2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Датчик 1T1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:00-08:30</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>08:30-09:00</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:00-09:30</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>09:30-10:00</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>10:00-10:30</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>10:30-11:00</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11:00-11:30</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:30-12:00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>12:00-12:30</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>12:30-13:00</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:00-13:30</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13:30-14:00</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>14:00-14:30</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:30-15:00</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>15:00-15:30</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>15:30-16:00</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>16:00-16:30</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>16:30-17:00</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>17:00-17:30</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>17:30-18:00</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>18:00-18:30</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>18:30-19:00</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>19:00-19:30</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>19:30-20:00</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>20:00-20:30</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>20:30-21:00</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>21:00-21:30</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>21:30-22:00</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>22:00-22:30</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>22:30-23:00</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>23:00-23:30</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2023-02-27</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>23:30-24:00</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>00:00-00:30</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>00:30-01:00</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>01:00-01:30</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>01:30-02:00</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>02:00-02:30</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>02:30-03:00</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>03:00-03:30</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>03:30-04:00</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>04:00-04:30</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>04:30-05:00</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>05:00-05:30</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>05:30-06:00</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>06:00-06:30</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>06:30-07:00</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>07:00-07:30</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>07:30-08:00</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>08:00-08:30</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>08:30-09:00</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>